<commit_message>
Refactored stored procedure for improved readability
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ting\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ting\Downloads\SSIS-ETL-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4282E3A-EF21-442C-8BF8-9C2EEAE6F468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A237FE43-764B-46F4-AA37-C87FB3A1F464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Source!$A$1:$G$34</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Source!$A$1:$G$36</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="156">
   <si>
     <t>UserID</t>
   </si>
@@ -475,6 +475,39 @@
   </si>
   <si>
     <t>2023-02-06</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>test1@example.com</t>
+  </si>
+  <si>
+    <t>29-07-2024 13:03:32</t>
+  </si>
+  <si>
+    <t>29-07-2024 13:04:20</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>test2@example.com</t>
+  </si>
+  <si>
+    <t>2024-07-29</t>
+  </si>
+  <si>
+    <t>2923-07-01</t>
   </si>
 </sst>
 </file>
@@ -585,16 +618,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F23B2B2C-47CD-4859-9066-D8E5B15EE230}" name="source__2" displayName="source__2" ref="A1:G34" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G34" xr:uid="{F23B2B2C-47CD-4859-9066-D8E5B15EE230}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F23B2B2C-47CD-4859-9066-D8E5B15EE230}" name="source__2" displayName="source__2" ref="A1:G36" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G36" xr:uid="{F23B2B2C-47CD-4859-9066-D8E5B15EE230}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{1AD70577-7A61-4A29-A080-6A464E1166D8}" uniqueName="1" name="UserID" queryTableFieldId="1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{68623AF3-E941-481F-9135-AD7F5043D65A}" uniqueName="2" name="FullName" queryTableFieldId="2" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{A232EB99-D4A2-4BD6-84E5-7807FBF02C89}" uniqueName="3" name="Age" queryTableFieldId="3" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{42BFCC70-29A7-4CDE-8763-AA48FEE55969}" uniqueName="4" name="Email" queryTableFieldId="4" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{EDFB8DC8-30B2-49B4-B6B5-DFEA0E97C45D}" uniqueName="5" name="RegistrationDate" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{292AE04C-B827-4079-A163-DFB3D609954B}" uniqueName="6" name="LastLoginDate" queryTableFieldId="6" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{CEC1099C-256A-4843-B533-07B154FB01B8}" uniqueName="7" name="PurchaseTotal" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{292AE04C-B827-4079-A163-DFB3D609954B}" uniqueName="6" name="LastLoginDate" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{CEC1099C-256A-4843-B533-07B154FB01B8}" uniqueName="7" name="PurchaseTotal" queryTableFieldId="7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -863,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A0909A-7C0F-4B6B-9724-9263FFB3A581}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1639,6 +1672,52 @@
       </c>
       <c r="G34" s="3">
         <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added index to improve lookup performance
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ting\Downloads\SSIS-ETL-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A237FE43-764B-46F4-AA37-C87FB3A1F464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C5D43A-FBB6-4BCD-83DD-017060DC0504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
     <t>2024-07-29</t>
   </si>
   <si>
-    <t>2923-07-01</t>
+    <t>2023-07-01</t>
   </si>
 </sst>
 </file>
@@ -899,7 +899,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added execution log to README
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ting\Downloads\SSIS-ETL-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C5D43A-FBB6-4BCD-83DD-017060DC0504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB326AD-C661-4875-AE18-36D30B3BF4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,12 +480,6 @@
     <t>139</t>
   </si>
   <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>test1@example.com</t>
-  </si>
-  <si>
     <t>29-07-2024 13:03:32</t>
   </si>
   <si>
@@ -498,16 +492,22 @@
     <t>140</t>
   </si>
   <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>test2@example.com</t>
-  </si>
-  <si>
     <t>2024-07-29</t>
   </si>
   <si>
     <t>2023-07-01</t>
+  </si>
+  <si>
+    <t>DateTimeFormat</t>
+  </si>
+  <si>
+    <t>datetimeformat@example.com</t>
+  </si>
+  <si>
+    <t>Incorrect Causality</t>
+  </si>
+  <si>
+    <t>incorrectcausality@example.com</t>
   </si>
 </sst>
 </file>
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A0909A-7C0F-4B6B-9724-9263FFB3A581}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1679,45 +1679,45 @@
         <v>145</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D35" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>